<commit_message>
graph is avilable with interactive options
</commit_message>
<xml_diff>
--- a/Data/Before preprocessing/rent_prices.xlsx
+++ b/Data/Before preprocessing/rent_prices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idansegal/Documents/Coding/aptVSstock/Data/Before preprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC16A1FE-3856-CE47-A2B0-215BF544336A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFFC98B-44F5-E044-8ECA-5BA02D49C59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7435" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7436" uniqueCount="385">
   <si>
     <t>קוד</t>
   </si>
@@ -1657,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1786"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A1683" workbookViewId="0">
-      <selection activeCell="D1791" sqref="D1791"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1707,7 +1707,9 @@
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C2" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>